<commit_message>
Added more details to the column definition of tables in the import script
</commit_message>
<xml_diff>
--- a/db_tools/acctg_export.xlsx
+++ b/db_tools/acctg_export.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgrammingPython\thanos_app\db_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7310BDFB-EFEB-4C4C-83F2-C4C609CCBB83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E2AB86-03C3-4667-AF8D-4BBB475A6544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="12" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="account_types" sheetId="1" r:id="rId1"/>
@@ -1718,9 +1718,6 @@
     <t>unit_price</t>
   </si>
   <si>
-    <t>line_total</t>
-  </si>
-  <si>
     <t>vendor_id</t>
   </si>
   <si>
@@ -1911,6 +1908,9 @@
   </si>
   <si>
     <t>2025-03-24 06:37:47</t>
+  </si>
+  <si>
+    <t>line_amount</t>
   </si>
 </sst>
 </file>
@@ -4292,7 +4292,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -4322,7 +4324,7 @@
         <v>528</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>559</v>
+        <v>623</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -4604,10 +4606,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>560</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>561</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>372</v>
@@ -4639,13 +4641,13 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D2" t="s">
         <v>375</v>
       </c>
       <c r="E2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F2">
         <v>535</v>
@@ -4671,7 +4673,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D3" t="s">
         <v>377</v>
@@ -4686,7 +4688,7 @@
         <v>210</v>
       </c>
       <c r="H3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="I3" t="s">
         <v>554</v>
@@ -4703,13 +4705,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F4">
         <v>2140</v>
@@ -4735,7 +4737,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D5" t="s">
         <v>383</v>
@@ -4750,7 +4752,7 @@
         <v>70</v>
       </c>
       <c r="H5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I5" t="s">
         <v>554</v>
@@ -4767,7 +4769,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D6" t="s">
         <v>538</v>
@@ -4782,7 +4784,7 @@
         <v>28</v>
       </c>
       <c r="H6" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I6" t="s">
         <v>554</v>
@@ -4799,7 +4801,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D7" t="s">
         <v>389</v>
@@ -4831,7 +4833,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D8" t="s">
         <v>539</v>
@@ -4863,7 +4865,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D9" t="s">
         <v>395</v>
@@ -4878,7 +4880,7 @@
         <v>245</v>
       </c>
       <c r="H9" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I9" t="s">
         <v>554</v>
@@ -4896,7 +4898,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -4905,7 +4909,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>556</v>
@@ -4926,7 +4930,7 @@
         <v>528</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>559</v>
+        <v>623</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -5199,7 +5203,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -5214,16 +5220,16 @@
         <v>555</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>578</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>579</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>166</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -5240,10 +5246,10 @@
         <v>2675</v>
       </c>
       <c r="E2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="G2">
         <v>3</v>
@@ -5263,10 +5269,10 @@
         <v>4815</v>
       </c>
       <c r="E3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -5286,10 +5292,10 @@
         <v>1070</v>
       </c>
       <c r="E4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -5309,10 +5315,10 @@
         <v>3210</v>
       </c>
       <c r="E5" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -5332,10 +5338,10 @@
         <v>5350</v>
       </c>
       <c r="E6" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F6" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -5355,10 +5361,10 @@
         <v>2140</v>
       </c>
       <c r="E7" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F7" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -5378,10 +5384,10 @@
         <v>3745</v>
       </c>
       <c r="E8" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F8" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="G8">
         <v>3</v>
@@ -5401,10 +5407,10 @@
         <v>1605</v>
       </c>
       <c r="E9" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F9" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -5431,19 +5437,19 @@
         <v>372</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>578</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>579</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>166</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -5460,10 +5466,10 @@
         <v>535</v>
       </c>
       <c r="E2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="G2">
         <v>3</v>
@@ -5483,10 +5489,10 @@
         <v>3210</v>
       </c>
       <c r="E3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -5506,10 +5512,10 @@
         <v>2140</v>
       </c>
       <c r="E4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -5529,10 +5535,10 @@
         <v>1070</v>
       </c>
       <c r="E5" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F5" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -5552,10 +5558,10 @@
         <v>428</v>
       </c>
       <c r="E6" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F6" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -5575,10 +5581,10 @@
         <v>1605</v>
       </c>
       <c r="E7" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F7" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -5598,10 +5604,10 @@
         <v>2675</v>
       </c>
       <c r="E8" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F8" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G8">
         <v>3</v>
@@ -5621,10 +5627,10 @@
         <v>3745</v>
       </c>
       <c r="E9" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F9" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -5639,7 +5645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -6880,7 +6886,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>372</v>
@@ -6889,25 +6895,25 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>614</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>615</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>462</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>616</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>617</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>17</v>
@@ -6930,7 +6936,7 @@
         <v>50000</v>
       </c>
       <c r="F2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -6939,7 +6945,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -6959,16 +6965,16 @@
         <v>-2000</v>
       </c>
       <c r="F3" t="s">
+        <v>621</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
         <v>622</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="L3" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -6988,7 +6994,7 @@
         <v>-500</v>
       </c>
       <c r="F4" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -6997,7 +7003,7 @@
         <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -7011,22 +7017,22 @@
         <v>377</v>
       </c>
       <c r="D5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E5">
         <v>-535</v>
       </c>
       <c r="F5" t="s">
+        <v>621</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
         <v>622</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -7046,7 +7052,7 @@
         <v>7500</v>
       </c>
       <c r="F6" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -7055,7 +7061,7 @@
         <v>4</v>
       </c>
       <c r="L6" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -7069,13 +7075,13 @@
         <v>378</v>
       </c>
       <c r="D7" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E7">
         <v>2675</v>
       </c>
       <c r="F7" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -7084,7 +7090,7 @@
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -7104,7 +7110,7 @@
         <v>-350</v>
       </c>
       <c r="F8" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -7113,7 +7119,7 @@
         <v>5</v>
       </c>
       <c r="L8" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -7127,22 +7133,22 @@
         <v>379</v>
       </c>
       <c r="D9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E9">
         <v>-3210</v>
       </c>
       <c r="F9" t="s">
+        <v>621</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9" t="s">
         <v>622</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>2</v>
-      </c>
-      <c r="L9" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -7156,13 +7162,13 @@
         <v>379</v>
       </c>
       <c r="D10" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E10">
         <v>4815</v>
       </c>
       <c r="F10" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -7171,7 +7177,7 @@
         <v>2</v>
       </c>
       <c r="L10" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -7191,7 +7197,7 @@
         <v>-12000</v>
       </c>
       <c r="F11" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -7200,7 +7206,7 @@
         <v>6</v>
       </c>
       <c r="L11" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -7220,7 +7226,7 @@
         <v>-5000</v>
       </c>
       <c r="F12" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -7229,7 +7235,7 @@
         <v>7</v>
       </c>
       <c r="L12" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -7249,7 +7255,7 @@
         <v>-2000</v>
       </c>
       <c r="F13" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -7258,7 +7264,7 @@
         <v>8</v>
       </c>
       <c r="L13" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -7272,13 +7278,13 @@
         <v>382</v>
       </c>
       <c r="D14" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E14">
         <v>-2140</v>
       </c>
       <c r="F14" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -7287,7 +7293,7 @@
         <v>3</v>
       </c>
       <c r="L14" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -7301,13 +7307,13 @@
         <v>382</v>
       </c>
       <c r="D15" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="E15">
         <v>1070</v>
       </c>
       <c r="F15" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -7316,7 +7322,7 @@
         <v>3</v>
       </c>
       <c r="L15" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
   </sheetData>

</xml_diff>